<commit_message>
perbarui template rks tunjuka langsung
</commit_message>
<xml_diff>
--- a/templates/PL-J-Lamp_2.xlsx
+++ b/templates/PL-J-Lamp_2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="45" windowWidth="9690" windowHeight="5985"/>
@@ -19,12 +19,6 @@
     <t>Lampiran : 2.</t>
   </si>
   <si>
-    <t>RINCIAN, JUMLAH DAN HARGA JASA BORONGAN PEKERJAAN.............</t>
-  </si>
-  <si>
-    <t>PT PLN (PERSERO) ...........................</t>
-  </si>
-  <si>
     <t>NOMOR     : ..................................................</t>
   </si>
   <si>
@@ -160,13 +154,19 @@
     <t xml:space="preserve">               *) Pilih yang sesuai.</t>
   </si>
   <si>
-    <t>RENCANA KERJA &amp; SYARAT-SYARAT (RKS) PEMILIHAN LANGSUNG</t>
+    <t>RENCANA KERJA &amp; SYARAT-SYARAT (RKS) PENUNJUKAN LANGSUNG</t>
+  </si>
+  <si>
+    <t>RINCIAN, JUMLAH DAN PEKERJAAN JASA .............</t>
+  </si>
+  <si>
+    <t>PT PLN (PERSERO) KANTOR PUSAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="8">
     <font>
       <sz val="10"/>
@@ -679,11 +679,6 @@
       <rgbColor rgb="00424242"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -762,7 +757,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -797,7 +791,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -973,11 +966,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1000,7 +993,7 @@
     </row>
     <row r="3" spans="2:8" ht="15">
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -1011,7 +1004,7 @@
     </row>
     <row r="4" spans="2:8" ht="15">
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1022,7 +1015,7 @@
     </row>
     <row r="5" spans="2:8" ht="15">
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1033,7 +1026,7 @@
     </row>
     <row r="6" spans="2:8" ht="15">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1044,7 +1037,7 @@
     </row>
     <row r="7" spans="2:8" ht="15">
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1067,32 +1060,32 @@
       <c r="D9" s="19"/>
       <c r="E9" s="42"/>
       <c r="F9" s="20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:8" ht="15">
       <c r="B10" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="E10" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="F10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="G10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>11</v>
-      </c>
       <c r="H10" s="33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1">
@@ -1115,10 +1108,10 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="44"/>
@@ -1138,11 +1131,11 @@
     <row r="15" spans="2:8">
       <c r="B15" s="18"/>
       <c r="C15" s="26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="7"/>
@@ -1151,7 +1144,7 @@
     <row r="16" spans="2:8">
       <c r="B16" s="18"/>
       <c r="C16" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="46"/>
@@ -1162,7 +1155,7 @@
     <row r="17" spans="2:8">
       <c r="B17" s="18"/>
       <c r="C17" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="46"/>
@@ -1173,7 +1166,7 @@
     <row r="18" spans="2:8">
       <c r="B18" s="18"/>
       <c r="C18" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="46"/>
@@ -1184,7 +1177,7 @@
     <row r="19" spans="2:8">
       <c r="B19" s="18"/>
       <c r="C19" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="46"/>
@@ -1195,7 +1188,7 @@
     <row r="20" spans="2:8">
       <c r="B20" s="18"/>
       <c r="C20" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="46"/>
@@ -1215,11 +1208,11 @@
     <row r="22" spans="2:8">
       <c r="B22" s="18"/>
       <c r="C22" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="7"/>
@@ -1228,7 +1221,7 @@
     <row r="23" spans="2:8">
       <c r="B23" s="18"/>
       <c r="C23" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="46"/>
@@ -1239,7 +1232,7 @@
     <row r="24" spans="2:8">
       <c r="B24" s="18"/>
       <c r="C24" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="46"/>
@@ -1250,7 +1243,7 @@
     <row r="25" spans="2:8">
       <c r="B25" s="18"/>
       <c r="C25" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="46"/>
@@ -1261,7 +1254,7 @@
     <row r="26" spans="2:8">
       <c r="B26" s="18"/>
       <c r="C26" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="46"/>
@@ -1272,7 +1265,7 @@
     <row r="27" spans="2:8">
       <c r="B27" s="18"/>
       <c r="C27" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="46"/>
@@ -1292,7 +1285,7 @@
     <row r="29" spans="2:8" ht="13.5" thickBot="1">
       <c r="B29" s="18"/>
       <c r="C29" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="46"/>
@@ -1311,10 +1304,10 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="46"/>
@@ -1334,11 +1327,11 @@
     <row r="33" spans="2:8">
       <c r="B33" s="18"/>
       <c r="C33" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="7"/>
@@ -1347,7 +1340,7 @@
     <row r="34" spans="2:8">
       <c r="B34" s="18"/>
       <c r="C34" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="46"/>
@@ -1367,7 +1360,7 @@
     <row r="36" spans="2:8" ht="13.5" thickBot="1">
       <c r="B36" s="18"/>
       <c r="C36" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="46"/>
@@ -1386,14 +1379,14 @@
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="7"/>
@@ -1402,7 +1395,7 @@
     <row r="39" spans="2:8">
       <c r="B39" s="18"/>
       <c r="C39" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="46"/>
@@ -1413,7 +1406,7 @@
     <row r="40" spans="2:8">
       <c r="B40" s="18"/>
       <c r="C40" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="46"/>
@@ -1433,7 +1426,7 @@
     <row r="42" spans="2:8" ht="13.5" thickBot="1">
       <c r="B42" s="18"/>
       <c r="C42" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="46"/>
@@ -1452,14 +1445,14 @@
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="7"/>
@@ -1468,7 +1461,7 @@
     <row r="45" spans="2:8">
       <c r="B45" s="18"/>
       <c r="C45" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="46"/>
@@ -1479,7 +1472,7 @@
     <row r="46" spans="2:8">
       <c r="B46" s="18"/>
       <c r="C46" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="46"/>
@@ -1490,7 +1483,7 @@
     <row r="47" spans="2:8">
       <c r="B47" s="18"/>
       <c r="C47" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="46"/>
@@ -1510,7 +1503,7 @@
     <row r="49" spans="2:8" ht="13.5" thickBot="1">
       <c r="B49" s="18"/>
       <c r="C49" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="46"/>
@@ -1529,10 +1522,10 @@
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="46"/>
@@ -1543,7 +1536,7 @@
     <row r="52" spans="2:8">
       <c r="B52" s="6"/>
       <c r="C52" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="46"/>
@@ -1554,7 +1547,7 @@
     <row r="53" spans="2:8">
       <c r="B53" s="6"/>
       <c r="C53" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="46"/>
@@ -1574,7 +1567,7 @@
     <row r="55" spans="2:8" ht="13.5" thickBot="1">
       <c r="B55" s="47"/>
       <c r="C55" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="45"/>
@@ -1584,7 +1577,7 @@
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1595,7 +1588,7 @@
     </row>
     <row r="57" spans="2:8" ht="13.5" thickBot="1">
       <c r="B57" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -1606,7 +1599,7 @@
     </row>
     <row r="58" spans="2:8" ht="13.5" thickBot="1">
       <c r="B58" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -1617,7 +1610,7 @@
     </row>
     <row r="59" spans="2:8" ht="14.25" thickTop="1" thickBot="1">
       <c r="B59" s="41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C59" s="38"/>
       <c r="D59" s="38"/>
@@ -1637,27 +1630,27 @@
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>